<commit_message>
Sửa lưu người dùng
</commit_message>
<xml_diff>
--- a/resources/PolyTest_DanhSachThiTemplate.xlsx
+++ b/resources/PolyTest_DanhSachThiTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School Projects\2025_K18_SD1802_PRO231\Assignment\PRO231_ExamApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School Projects\2025_K18_SD1802_PRO231\Assignment\PRO231_ExamApp\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3262686-6BD5-414A-AC3C-A29AB77938BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F3B0C4-042C-4CD1-A135-7F18898D1781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19665" yWindow="4695" windowWidth="14145" windowHeight="9045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="285" yWindow="2175" windowWidth="18960" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thong Tin" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>MaThiSinh</t>
   </si>
   <si>
     <t>TS001</t>
+  </si>
+  <si>
+    <t>TS003</t>
   </si>
 </sst>
 </file>
@@ -89,12 +92,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -105,6 +111,26 @@
     <cellStyle name="Table Text" xfId="3" xr:uid="{888AE7D8-C4DF-4345-B361-7FC4356C86C3}"/>
   </cellStyles>
   <dxfs count="8">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -137,26 +163,6 @@
           <color theme="4" tint="-0.749992370372631"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -307,10 +313,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8F7A7EF5-B089-4716-BD92-FB40E5E39317}" name="MultipleChoiceData3" displayName="MultipleChoiceData3" ref="A1:A2" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" totalsRowDxfId="2" headerRowCellStyle="Header Row">
-  <autoFilter ref="A1:A2" xr:uid="{8F7A7EF5-B089-4716-BD92-FB40E5E39317}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8F7A7EF5-B089-4716-BD92-FB40E5E39317}" name="MultipleChoiceData3" displayName="MultipleChoiceData3" ref="A1:A3" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" totalsRowDxfId="2" headerRowCellStyle="Header Row">
+  <autoFilter ref="A1:A3" xr:uid="{8F7A7EF5-B089-4716-BD92-FB40E5E39317}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{A09D6441-B594-4101-BF76-D433E4EB42EE}" name="MaThiSinh" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Date"/>
+    <tableColumn id="1" xr3:uid="{A09D6441-B594-4101-BF76-D433E4EB42EE}" name="MaThiSinh" dataDxfId="0" totalsRowDxfId="1" dataCellStyle="Date"/>
   </tableColumns>
   <tableStyleInfo name="Business Table" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -584,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,6 +616,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Date in this column under this heading" sqref="A1" xr:uid="{FD054FFF-883E-4599-9086-0768D060239E}"/>

</xml_diff>